<commit_message>
added table in documentation and tried to calculate the frquency
</commit_message>
<xml_diff>
--- a/code/experiments/record6/record6.xlsx
+++ b/code/experiments/record6/record6.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentinbossi/Downloads/record6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentinbossi/Documents/git/pa17_cogsworth/code/experiments/record6/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -5429,11 +5429,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-619223840"/>
-        <c:axId val="-619310240"/>
+        <c:axId val="1532306800"/>
+        <c:axId val="1625638960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-619223840"/>
+        <c:axId val="1532306800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5475,7 +5475,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-619310240"/>
+        <c:crossAx val="1625638960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5483,7 +5483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-619310240"/>
+        <c:axId val="1625638960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5533,7 +5533,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-619223840"/>
+        <c:crossAx val="1532306800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6470,8 +6470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J863"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G860" sqref="G860"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6714,6 +6714,9 @@
       <c r="D10">
         <v>88645</v>
       </c>
+      <c r="E10">
+        <v>88645</v>
+      </c>
       <c r="F10">
         <v>1429401</v>
       </c>
@@ -16742,7 +16745,7 @@
         <v>9529338</v>
       </c>
     </row>
-    <row r="849" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="849" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A849" s="1">
         <v>1630</v>
       </c>
@@ -16753,7 +16756,7 @@
         <v>9540418</v>
       </c>
     </row>
-    <row r="850" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="850" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A850">
         <v>3624</v>
       </c>
@@ -16764,7 +16767,7 @@
         <v>9551500</v>
       </c>
     </row>
-    <row r="851" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="851" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A851">
         <v>1888</v>
       </c>
@@ -16775,7 +16778,7 @@
         <v>9562579</v>
       </c>
     </row>
-    <row r="852" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="852" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A852">
         <v>3554</v>
       </c>
@@ -16786,7 +16789,7 @@
         <v>9573660</v>
       </c>
     </row>
-    <row r="853" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="853" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A853">
         <v>3838</v>
       </c>
@@ -16797,7 +16800,7 @@
         <v>9584742</v>
       </c>
     </row>
-    <row r="854" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="854" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A854">
         <v>2056</v>
       </c>
@@ -16808,7 +16811,7 @@
         <v>9595821</v>
       </c>
     </row>
-    <row r="855" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="855" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A855">
         <v>2426</v>
       </c>
@@ -16819,7 +16822,7 @@
         <v>9606902</v>
       </c>
     </row>
-    <row r="856" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="856" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A856">
         <v>2936</v>
       </c>
@@ -16830,7 +16833,7 @@
         <v>9617985</v>
       </c>
     </row>
-    <row r="857" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="857" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A857">
         <v>3606</v>
       </c>
@@ -16841,7 +16844,7 @@
         <v>9629063</v>
       </c>
     </row>
-    <row r="858" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="858" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A858">
         <v>1800</v>
       </c>
@@ -16852,7 +16855,7 @@
         <v>9640143</v>
       </c>
     </row>
-    <row r="859" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="859" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A859">
         <v>1032</v>
       </c>
@@ -16863,7 +16866,7 @@
         <v>9651224</v>
       </c>
     </row>
-    <row r="860" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="860" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A860">
         <v>38</v>
       </c>
@@ -16876,8 +16879,19 @@
       <c r="D860">
         <v>9662305</v>
       </c>
-    </row>
-    <row r="861" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E860">
+        <v>9662305</v>
+      </c>
+      <c r="F860">
+        <f>E860-E10</f>
+        <v>9573660</v>
+      </c>
+      <c r="G860">
+        <f>F860/59</f>
+        <v>162265.42372881356</v>
+      </c>
+    </row>
+    <row r="861" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A861">
         <v>868</v>
       </c>
@@ -16888,7 +16902,7 @@
         <v>9673385</v>
       </c>
     </row>
-    <row r="862" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="862" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A862">
         <v>1752</v>
       </c>
@@ -16899,7 +16913,7 @@
         <v>9684469</v>
       </c>
     </row>
-    <row r="863" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="863" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A863">
         <v>2662</v>
       </c>

</xml_diff>

<commit_message>
changed file content to english
</commit_message>
<xml_diff>
--- a/code/experiments/record6/record6.xlsx
+++ b/code/experiments/record6/record6.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentinbossi/Documents/git/pa17_cogsworth/code/experiments/record6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Linda/Documents/Bildung/Studium/ZHAW/Semester_5/PA/pa17_cogsworth/code/experiments/record6/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="6980" yWindow="480" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,28 +35,28 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>ausreisser timestamps</t>
-  </si>
-  <si>
-    <t>halbe periode</t>
-  </si>
-  <si>
-    <t>ganze periode</t>
-  </si>
-  <si>
     <t>hertz</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>hertz im schnitt</t>
-  </si>
-  <si>
     <t>xSumAbs</t>
   </si>
   <si>
     <t>ySumAbs</t>
+  </si>
+  <si>
+    <t>timestamp stillstand</t>
+  </si>
+  <si>
+    <t>half period</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>hertz average</t>
   </si>
 </sst>
 </file>
@@ -5429,11 +5429,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1532306800"/>
-        <c:axId val="1625638960"/>
+        <c:axId val="-1722364256"/>
+        <c:axId val="-1722361936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1532306800"/>
+        <c:axId val="-1722364256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5475,7 +5475,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1625638960"/>
+        <c:crossAx val="-1722361936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5483,7 +5483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1625638960"/>
+        <c:axId val="-1722361936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5533,7 +5533,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1532306800"/>
+        <c:crossAx val="-1722364256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6470,8 +6470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J863"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G860" sqref="G860"/>
+    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6485,28 +6485,28 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
       <c r="J1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -6527,7 +6527,7 @@
         <v>166210</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J2" s="2">
         <f>SUM(I:I)/29</f>
@@ -6578,7 +6578,7 @@
         <v>177290</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -6625,7 +6625,7 @@
         <v>177289</v>
       </c>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -6672,7 +6672,7 @@
         <v>166210</v>
       </c>
       <c r="H8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6714,9 +6714,6 @@
       <c r="D10">
         <v>88645</v>
       </c>
-      <c r="E10">
-        <v>88645</v>
-      </c>
       <c r="F10">
         <v>1429401</v>
       </c>
@@ -6725,7 +6722,7 @@
         <v>166209</v>
       </c>
       <c r="H10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -6772,7 +6769,7 @@
         <v>166209</v>
       </c>
       <c r="H12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -6819,7 +6816,7 @@
         <v>166209</v>
       </c>
       <c r="H14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -6866,7 +6863,7 @@
         <v>166210</v>
       </c>
       <c r="H16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -6913,7 +6910,7 @@
         <v>166209</v>
       </c>
       <c r="H18" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -6960,7 +6957,7 @@
         <v>166209</v>
       </c>
       <c r="H20" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -7007,7 +7004,7 @@
         <v>166210</v>
       </c>
       <c r="H22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -7054,7 +7051,7 @@
         <v>166211</v>
       </c>
       <c r="H24" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -7104,7 +7101,7 @@
         <v>166209</v>
       </c>
       <c r="H26" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -7151,7 +7148,7 @@
         <v>166208</v>
       </c>
       <c r="H28" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -7198,7 +7195,7 @@
         <v>166209</v>
       </c>
       <c r="H30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -7245,7 +7242,7 @@
         <v>166209</v>
       </c>
       <c r="H32" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -7292,7 +7289,7 @@
         <v>166210</v>
       </c>
       <c r="H34" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -7339,7 +7336,7 @@
         <v>166210</v>
       </c>
       <c r="H36" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -7386,7 +7383,7 @@
         <v>166209</v>
       </c>
       <c r="H38" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -7436,7 +7433,7 @@
         <v>166210</v>
       </c>
       <c r="H40" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -7483,7 +7480,7 @@
         <v>166210</v>
       </c>
       <c r="H42" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -7530,7 +7527,7 @@
         <v>166209</v>
       </c>
       <c r="H44" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -7577,7 +7574,7 @@
         <v>166208</v>
       </c>
       <c r="H46" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -7624,7 +7621,7 @@
         <v>177288</v>
       </c>
       <c r="H48" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -7671,7 +7668,7 @@
         <v>166209</v>
       </c>
       <c r="H50" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
@@ -7718,7 +7715,7 @@
         <v>166208</v>
       </c>
       <c r="H52" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
@@ -7765,7 +7762,7 @@
         <v>166209</v>
       </c>
       <c r="H54" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -7815,7 +7812,7 @@
         <v>132988</v>
       </c>
       <c r="H56" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
@@ -7862,7 +7859,7 @@
         <v>166210</v>
       </c>
       <c r="H58" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -7909,7 +7906,7 @@
         <v>-9662305</v>
       </c>
       <c r="H60" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -16745,7 +16742,7 @@
         <v>9529338</v>
       </c>
     </row>
-    <row r="849" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="849" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A849" s="1">
         <v>1630</v>
       </c>
@@ -16756,7 +16753,7 @@
         <v>9540418</v>
       </c>
     </row>
-    <row r="850" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="850" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A850">
         <v>3624</v>
       </c>
@@ -16767,7 +16764,7 @@
         <v>9551500</v>
       </c>
     </row>
-    <row r="851" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="851" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A851">
         <v>1888</v>
       </c>
@@ -16778,7 +16775,7 @@
         <v>9562579</v>
       </c>
     </row>
-    <row r="852" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="852" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A852">
         <v>3554</v>
       </c>
@@ -16789,7 +16786,7 @@
         <v>9573660</v>
       </c>
     </row>
-    <row r="853" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="853" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A853">
         <v>3838</v>
       </c>
@@ -16800,7 +16797,7 @@
         <v>9584742</v>
       </c>
     </row>
-    <row r="854" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="854" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A854">
         <v>2056</v>
       </c>
@@ -16811,7 +16808,7 @@
         <v>9595821</v>
       </c>
     </row>
-    <row r="855" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="855" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A855">
         <v>2426</v>
       </c>
@@ -16822,7 +16819,7 @@
         <v>9606902</v>
       </c>
     </row>
-    <row r="856" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="856" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A856">
         <v>2936</v>
       </c>
@@ -16833,7 +16830,7 @@
         <v>9617985</v>
       </c>
     </row>
-    <row r="857" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="857" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A857">
         <v>3606</v>
       </c>
@@ -16844,7 +16841,7 @@
         <v>9629063</v>
       </c>
     </row>
-    <row r="858" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="858" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A858">
         <v>1800</v>
       </c>
@@ -16855,7 +16852,7 @@
         <v>9640143</v>
       </c>
     </row>
-    <row r="859" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="859" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A859">
         <v>1032</v>
       </c>
@@ -16866,7 +16863,7 @@
         <v>9651224</v>
       </c>
     </row>
-    <row r="860" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="860" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A860">
         <v>38</v>
       </c>
@@ -16879,19 +16876,8 @@
       <c r="D860">
         <v>9662305</v>
       </c>
-      <c r="E860">
-        <v>9662305</v>
-      </c>
-      <c r="F860">
-        <f>E860-E10</f>
-        <v>9573660</v>
-      </c>
-      <c r="G860">
-        <f>F860/59</f>
-        <v>162265.42372881356</v>
-      </c>
-    </row>
-    <row r="861" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="861" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A861">
         <v>868</v>
       </c>
@@ -16902,7 +16888,7 @@
         <v>9673385</v>
       </c>
     </row>
-    <row r="862" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="862" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A862">
         <v>1752</v>
       </c>
@@ -16913,7 +16899,7 @@
         <v>9684469</v>
       </c>
     </row>
-    <row r="863" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="863" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A863">
         <v>2662</v>
       </c>

</xml_diff>